<commit_message>
opdaterede ark med grupper
</commit_message>
<xml_diff>
--- a/Estimering/fastepriser.xlsx
+++ b/Estimering/fastepriser.xlsx
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rasmuskaslund/Documents/GitHub/SpecialeJR /Estimering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD25B7F-C134-9140-9F9F-0C16EC5386E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52F2CE6-C48B-E84E-936A-06632987F88D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="1400" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FU05" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="91">
   <si>
     <t>1994</t>
   </si>
@@ -258,6 +268,42 @@
   <si>
     <t>Kategori</t>
   </si>
+  <si>
+    <t>MAKRO_gruppe</t>
+  </si>
+  <si>
+    <t>Egen_gruppe</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Varer</t>
+  </si>
+  <si>
+    <t>Fødevarer</t>
+  </si>
+  <si>
+    <t>Andre varer</t>
+  </si>
+  <si>
+    <t>Bolig</t>
+  </si>
+  <si>
+    <t>Energi</t>
+  </si>
+  <si>
+    <t>Tjenester</t>
+  </si>
+  <si>
+    <t>Biler</t>
+  </si>
+  <si>
+    <t>Off transport</t>
+  </si>
+  <si>
+    <t>Turisme</t>
+  </si>
 </sst>
 </file>
 
@@ -298,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -306,6 +352,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA283"/>
+  <dimension ref="A1:AC283"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1:AC283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -620,7 +670,7 @@
     <col min="2" max="27" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
@@ -702,8 +752,14 @@
       <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
@@ -785,8 +841,14 @@
       <c r="AA2" s="2">
         <v>316611</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -868,8 +930,14 @@
       <c r="AA3" s="2">
         <v>33004</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -951,8 +1019,14 @@
       <c r="AA4" s="2">
         <v>3644</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1034,8 +1108,14 @@
       <c r="AA5" s="2">
         <v>4773</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1117,8 +1197,14 @@
       <c r="AA6" s="2">
         <v>1980</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -1200,8 +1286,14 @@
       <c r="AA7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC7" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1283,8 +1375,14 @@
       <c r="AA8" s="2">
         <v>10883</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC8" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1366,8 +1464,14 @@
       <c r="AA9" s="2">
         <v>1993</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC9" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1449,8 +1553,14 @@
       <c r="AA10" s="2">
         <v>28049</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC10" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1532,8 +1642,14 @@
       <c r="AA11" s="2">
         <v>39525</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC11" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -1615,8 +1731,14 @@
       <c r="AA12" s="2">
         <v>2843</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC12" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1698,8 +1820,14 @@
       <c r="AA13" s="2">
         <v>8992</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC13" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -1781,8 +1909,14 @@
       <c r="AA14" s="2">
         <v>24445</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC14" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1864,8 +1998,14 @@
       <c r="AA15" s="2">
         <v>6522</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB15" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC15" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1947,8 +2087,14 @@
       <c r="AA16" s="2">
         <v>1113</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC16" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -2030,8 +2176,14 @@
       <c r="AA17" s="2">
         <v>2386</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC17" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -2113,8 +2265,14 @@
       <c r="AA18" s="2">
         <v>1784</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC18" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -2196,8 +2354,14 @@
       <c r="AA19" s="2">
         <v>1374</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC19" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -2279,8 +2443,14 @@
       <c r="AA20" s="2">
         <v>3183</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC20" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -2362,8 +2532,14 @@
       <c r="AA21" s="2">
         <v>3581</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC21" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -2445,8 +2621,14 @@
       <c r="AA22" s="2">
         <v>3830</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC22" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>46</v>
       </c>
@@ -2528,8 +2710,14 @@
       <c r="AA23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC23" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -2611,8 +2799,14 @@
       <c r="AA24" s="2">
         <v>18466</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC24" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -2694,8 +2888,14 @@
       <c r="AA25" s="2">
         <v>20428</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC25" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -2777,8 +2977,14 @@
       <c r="AA26" s="2">
         <v>5469</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB26" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC26" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -2860,8 +3066,14 @@
       <c r="AA27" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC27" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -2943,8 +3155,14 @@
       <c r="AA28" s="2">
         <v>1736</v>
       </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC28" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
@@ -3026,8 +3244,14 @@
       <c r="AA29" s="2">
         <v>7633</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC29" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -3109,8 +3333,14 @@
       <c r="AA30" s="2">
         <v>4289</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB30" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC30" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
@@ -3192,8 +3422,14 @@
       <c r="AA31" s="2">
         <v>2060</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB31" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC31" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
@@ -3275,8 +3511,14 @@
       <c r="AA32" s="2">
         <v>7096</v>
       </c>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB32" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC32" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>56</v>
       </c>
@@ -3358,8 +3600,14 @@
       <c r="AA33" s="2">
         <v>9996</v>
       </c>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB33" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC33" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
@@ -3441,8 +3689,14 @@
       <c r="AA34" s="2">
         <v>2109</v>
       </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC34" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -3524,8 +3778,14 @@
       <c r="AA35" s="2">
         <v>5585</v>
       </c>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB35" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC35" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>59</v>
       </c>
@@ -3607,8 +3867,14 @@
       <c r="AA36" s="2">
         <v>690</v>
       </c>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB36" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC36" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>60</v>
       </c>
@@ -3690,8 +3956,14 @@
       <c r="AA37" s="2">
         <v>528</v>
       </c>
-    </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC37" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>61</v>
       </c>
@@ -3773,8 +4045,14 @@
       <c r="AA38" s="2">
         <v>146</v>
       </c>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC38" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>62</v>
       </c>
@@ -3856,8 +4134,14 @@
       <c r="AA39" s="2">
         <v>174</v>
       </c>
-    </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB39" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC39" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>63</v>
       </c>
@@ -3939,8 +4223,14 @@
       <c r="AA40" s="2">
         <v>14388</v>
       </c>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC40" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>64</v>
       </c>
@@ -4022,8 +4312,14 @@
       <c r="AA41" s="2">
         <v>4063</v>
       </c>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB41" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC41" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -4105,8 +4401,14 @@
       <c r="AA42" s="2">
         <v>6540</v>
       </c>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB42" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC42" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>66</v>
       </c>
@@ -4188,8 +4490,14 @@
       <c r="AA43" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB43" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC43" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>67</v>
       </c>
@@ -4271,8 +4579,14 @@
       <c r="AA44" s="2">
         <v>1953</v>
       </c>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB44" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC44" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>68</v>
       </c>
@@ -4354,8 +4668,14 @@
       <c r="AA45" s="2">
         <v>3652</v>
       </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB45" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC45" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>69</v>
       </c>
@@ -4437,8 +4757,14 @@
       <c r="AA46" s="2">
         <v>14500</v>
       </c>
-    </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB46" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC46" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>70</v>
       </c>
@@ -4520,8 +4846,14 @@
       <c r="AA47" s="2">
         <v>530</v>
       </c>
-    </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB47" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC47" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>71</v>
       </c>
@@ -4603,8 +4935,14 @@
       <c r="AA48" s="2">
         <v>642</v>
       </c>
-    </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB48" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC48" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>72</v>
       </c>
@@ -4686,8 +5024,14 @@
       <c r="AA49" s="2">
         <v>163874</v>
       </c>
-    </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB49" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC49" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>26</v>
       </c>
@@ -4769,8 +5113,14 @@
       <c r="AA50" s="2">
         <v>17479</v>
       </c>
-    </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB50" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC50" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>27</v>
       </c>
@@ -4852,8 +5202,14 @@
       <c r="AA51" s="2">
         <v>2124</v>
       </c>
-    </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB51" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC51" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>28</v>
       </c>
@@ -4935,8 +5291,14 @@
       <c r="AA52" s="2">
         <v>2413</v>
       </c>
-    </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB52" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC52" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>29</v>
       </c>
@@ -5018,8 +5380,14 @@
       <c r="AA53" s="2">
         <v>1870</v>
       </c>
-    </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB53" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC53" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>30</v>
       </c>
@@ -5101,8 +5469,14 @@
       <c r="AA54" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB54" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC54" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>31</v>
       </c>
@@ -5184,8 +5558,14 @@
       <c r="AA55" s="2">
         <v>5375</v>
       </c>
-    </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB55" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC55" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>32</v>
       </c>
@@ -5267,8 +5647,14 @@
       <c r="AA56" s="2">
         <v>947</v>
       </c>
-    </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB56" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC56" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>33</v>
       </c>
@@ -5350,8 +5736,14 @@
       <c r="AA57" s="2">
         <v>39263</v>
       </c>
-    </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB57" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC57" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>34</v>
       </c>
@@ -5433,8 +5825,14 @@
       <c r="AA58" s="2">
         <v>5024</v>
       </c>
-    </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB58" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC58" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>35</v>
       </c>
@@ -5516,8 +5914,14 @@
       <c r="AA59" s="2">
         <v>641</v>
       </c>
-    </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB59" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC59" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>36</v>
       </c>
@@ -5599,8 +6003,14 @@
       <c r="AA60" s="2">
         <v>4758</v>
       </c>
-    </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB60" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC60" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>37</v>
       </c>
@@ -5682,8 +6092,14 @@
       <c r="AA61" s="2">
         <v>18532</v>
       </c>
-    </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB61" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC61" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>38</v>
       </c>
@@ -5765,8 +6181,14 @@
       <c r="AA62" s="2">
         <v>2420</v>
       </c>
-    </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB62" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC62" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>39</v>
       </c>
@@ -5848,8 +6270,14 @@
       <c r="AA63" s="2">
         <v>804</v>
       </c>
-    </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB63" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC63" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>40</v>
       </c>
@@ -5931,8 +6359,14 @@
       <c r="AA64" s="2">
         <v>1263</v>
       </c>
-    </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB64" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC64" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>41</v>
       </c>
@@ -6014,8 +6448,14 @@
       <c r="AA65" s="2">
         <v>801</v>
       </c>
-    </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB65" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC65" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>42</v>
       </c>
@@ -6097,8 +6537,14 @@
       <c r="AA66" s="2">
         <v>591</v>
       </c>
-    </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB66" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC66" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>43</v>
       </c>
@@ -6180,8 +6626,14 @@
       <c r="AA67" s="2">
         <v>1271</v>
       </c>
-    </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB67" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC67" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>44</v>
       </c>
@@ -6263,8 +6715,14 @@
       <c r="AA68" s="2">
         <v>3041</v>
       </c>
-    </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB68" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC68" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>45</v>
       </c>
@@ -6346,8 +6804,14 @@
       <c r="AA69" s="2">
         <v>1912</v>
       </c>
-    </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB69" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC69" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>46</v>
       </c>
@@ -6429,8 +6893,14 @@
       <c r="AA70" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB70" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC70" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>47</v>
       </c>
@@ -6512,8 +6982,14 @@
       <c r="AA71" s="2">
         <v>4154</v>
       </c>
-    </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB71" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC71" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>48</v>
       </c>
@@ -6595,8 +7071,14 @@
       <c r="AA72" s="2">
         <v>5948</v>
       </c>
-    </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB72" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC72" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>49</v>
       </c>
@@ -6678,8 +7160,14 @@
       <c r="AA73" s="2">
         <v>3406</v>
       </c>
-    </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB73" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC73" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>50</v>
       </c>
@@ -6761,8 +7249,14 @@
       <c r="AA74" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB74" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC74" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>51</v>
       </c>
@@ -6844,8 +7338,14 @@
       <c r="AA75" s="2">
         <v>997</v>
       </c>
-    </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB75" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC75" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>52</v>
       </c>
@@ -6927,8 +7427,14 @@
       <c r="AA76" s="2">
         <v>4596</v>
       </c>
-    </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB76" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC76" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>53</v>
       </c>
@@ -7010,8 +7516,14 @@
       <c r="AA77" s="2">
         <v>2564</v>
       </c>
-    </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB77" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC77" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>54</v>
       </c>
@@ -7093,8 +7605,14 @@
       <c r="AA78" s="2">
         <v>101</v>
       </c>
-    </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB78" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC78" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>55</v>
       </c>
@@ -7176,8 +7694,14 @@
       <c r="AA79" s="2">
         <v>3405</v>
       </c>
-    </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB79" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC79" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>56</v>
       </c>
@@ -7259,8 +7783,14 @@
       <c r="AA80" s="2">
         <v>5609</v>
       </c>
-    </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB80" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC80" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>57</v>
       </c>
@@ -7342,8 +7872,14 @@
       <c r="AA81" s="2">
         <v>1321</v>
       </c>
-    </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB81" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC81" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>58</v>
       </c>
@@ -7425,8 +7961,14 @@
       <c r="AA82" s="2">
         <v>992</v>
       </c>
-    </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB82" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC82" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>59</v>
       </c>
@@ -7508,8 +8050,14 @@
       <c r="AA83" s="2">
         <v>130</v>
       </c>
-    </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB83" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC83" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>60</v>
       </c>
@@ -7591,8 +8139,14 @@
       <c r="AA84" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB84" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC84" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>61</v>
       </c>
@@ -7674,8 +8228,14 @@
       <c r="AA85" s="2">
         <v>617</v>
       </c>
-    </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB85" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC85" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>62</v>
       </c>
@@ -7757,8 +8317,14 @@
       <c r="AA86" s="2">
         <v>111</v>
       </c>
-    </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB86" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC86" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>63</v>
       </c>
@@ -7840,8 +8406,14 @@
       <c r="AA87" s="2">
         <v>6836</v>
       </c>
-    </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB87" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC87" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>64</v>
       </c>
@@ -7923,8 +8495,14 @@
       <c r="AA88" s="2">
         <v>1407</v>
       </c>
-    </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB88" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC88" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>65</v>
       </c>
@@ -8006,8 +8584,14 @@
       <c r="AA89" s="2">
         <v>3848</v>
       </c>
-    </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB89" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC89" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>66</v>
       </c>
@@ -8089,8 +8673,14 @@
       <c r="AA90" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB90" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC90" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>67</v>
       </c>
@@ -8172,8 +8762,14 @@
       <c r="AA91" s="2">
         <v>1356</v>
       </c>
-    </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB91" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC91" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>68</v>
       </c>
@@ -8255,8 +8851,14 @@
       <c r="AA92" s="2">
         <v>554</v>
       </c>
-    </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB92" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC92" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>69</v>
       </c>
@@ -8338,8 +8940,14 @@
       <c r="AA93" s="2">
         <v>4901</v>
       </c>
-    </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB93" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC93" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>70</v>
       </c>
@@ -8421,8 +9029,14 @@
       <c r="AA94" s="2">
         <v>149</v>
       </c>
-    </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB94" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC94" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="95" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>71</v>
       </c>
@@ -8504,8 +9118,14 @@
       <c r="AA95" s="2">
         <v>313</v>
       </c>
-    </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB95" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC95" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>74</v>
       </c>
@@ -8587,8 +9207,14 @@
       <c r="AA96" s="2">
         <v>219140</v>
       </c>
-    </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB96" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC96" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="97" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>26</v>
       </c>
@@ -8670,8 +9296,14 @@
       <c r="AA97" s="2">
         <v>24579</v>
       </c>
-    </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB97" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC97" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="98" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>27</v>
       </c>
@@ -8753,8 +9385,14 @@
       <c r="AA98" s="2">
         <v>3051</v>
       </c>
-    </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB98" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC98" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="99" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>28</v>
       </c>
@@ -8836,8 +9474,14 @@
       <c r="AA99" s="2">
         <v>3096</v>
       </c>
-    </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB99" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC99" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="100" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>29</v>
       </c>
@@ -8919,8 +9563,14 @@
       <c r="AA100" s="2">
         <v>2028</v>
       </c>
-    </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB100" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC100" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="101" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>30</v>
       </c>
@@ -9002,8 +9652,14 @@
       <c r="AA101" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB101" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC101" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="102" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>31</v>
       </c>
@@ -9085,8 +9741,14 @@
       <c r="AA102" s="2">
         <v>7996</v>
       </c>
-    </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB102" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC102" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="103" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>32</v>
       </c>
@@ -9168,8 +9830,14 @@
       <c r="AA103" s="2">
         <v>1509</v>
       </c>
-    </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB103" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC103" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="104" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>33</v>
       </c>
@@ -9251,8 +9919,14 @@
       <c r="AA104" s="2">
         <v>36165</v>
       </c>
-    </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB104" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC104" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="105" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>34</v>
       </c>
@@ -9334,8 +10008,14 @@
       <c r="AA105" s="2">
         <v>17942</v>
       </c>
-    </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB105" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC105" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="106" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>35</v>
       </c>
@@ -9417,8 +10097,14 @@
       <c r="AA106" s="2">
         <v>2121</v>
       </c>
-    </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB106" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC106" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="107" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>36</v>
       </c>
@@ -9500,8 +10186,14 @@
       <c r="AA107" s="2">
         <v>7046</v>
       </c>
-    </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB107" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC107" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="108" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>37</v>
       </c>
@@ -9583,8 +10275,14 @@
       <c r="AA108" s="2">
         <v>21277</v>
       </c>
-    </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB108" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC108" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="109" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>38</v>
       </c>
@@ -9666,8 +10364,14 @@
       <c r="AA109" s="2">
         <v>2836</v>
       </c>
-    </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB109" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC109" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>39</v>
       </c>
@@ -9749,8 +10453,14 @@
       <c r="AA110" s="2">
         <v>517</v>
       </c>
-    </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB110" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC110" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>40</v>
       </c>
@@ -9832,8 +10542,14 @@
       <c r="AA111" s="2">
         <v>1210</v>
       </c>
-    </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB111" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC111" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>41</v>
       </c>
@@ -9915,8 +10631,14 @@
       <c r="AA112" s="2">
         <v>1462</v>
       </c>
-    </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB112" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC112" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="113" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>42</v>
       </c>
@@ -9998,8 +10720,14 @@
       <c r="AA113" s="2">
         <v>551</v>
       </c>
-    </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB113" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC113" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="114" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>43</v>
       </c>
@@ -10081,8 +10809,14 @@
       <c r="AA114" s="2">
         <v>1968</v>
       </c>
-    </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB114" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC114" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="115" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>44</v>
       </c>
@@ -10164,8 +10898,14 @@
       <c r="AA115" s="2">
         <v>2207</v>
       </c>
-    </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB115" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC115" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="116" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>45</v>
       </c>
@@ -10247,8 +10987,14 @@
       <c r="AA116" s="2">
         <v>3204</v>
       </c>
-    </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB116" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC116" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="117" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>46</v>
       </c>
@@ -10330,8 +11076,14 @@
       <c r="AA117" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB117" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC117" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="118" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>47</v>
       </c>
@@ -10413,8 +11165,14 @@
       <c r="AA118" s="2">
         <v>7495</v>
       </c>
-    </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB118" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC118" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="119" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>48</v>
       </c>
@@ -10496,8 +11254,14 @@
       <c r="AA119" s="2">
         <v>10621</v>
       </c>
-    </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB119" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC119" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="120" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>49</v>
       </c>
@@ -10579,8 +11343,14 @@
       <c r="AA120" s="2">
         <v>3222</v>
       </c>
-    </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB120" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC120" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="121" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>50</v>
       </c>
@@ -10662,8 +11432,14 @@
       <c r="AA121" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB121" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC121" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="122" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>51</v>
       </c>
@@ -10745,8 +11521,14 @@
       <c r="AA122" s="2">
         <v>1170</v>
       </c>
-    </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB122" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC122" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="123" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>52</v>
       </c>
@@ -10828,8 +11610,14 @@
       <c r="AA123" s="2">
         <v>6480</v>
       </c>
-    </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB123" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC123" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="124" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>53</v>
       </c>
@@ -10911,8 +11699,14 @@
       <c r="AA124" s="2">
         <v>2979</v>
       </c>
-    </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB124" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC124" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>54</v>
       </c>
@@ -10994,8 +11788,14 @@
       <c r="AA125" s="2">
         <v>237</v>
       </c>
-    </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB125" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC125" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="126" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>55</v>
       </c>
@@ -11077,8 +11877,14 @@
       <c r="AA126" s="2">
         <v>6149</v>
       </c>
-    </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB126" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC126" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="127" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>56</v>
       </c>
@@ -11160,8 +11966,14 @@
       <c r="AA127" s="2">
         <v>7990</v>
       </c>
-    </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB127" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC127" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="128" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>57</v>
       </c>
@@ -11243,8 +12055,14 @@
       <c r="AA128" s="2">
         <v>1916</v>
       </c>
-    </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB128" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC128" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="129" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>58</v>
       </c>
@@ -11326,8 +12144,14 @@
       <c r="AA129" s="2">
         <v>4101</v>
       </c>
-    </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB129" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC129" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="130" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>59</v>
       </c>
@@ -11409,8 +12233,14 @@
       <c r="AA130" s="2">
         <v>90</v>
       </c>
-    </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB130" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC130" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="131" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>60</v>
       </c>
@@ -11492,8 +12322,14 @@
       <c r="AA131" s="2">
         <v>73</v>
       </c>
-    </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB131" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC131" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="132" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>61</v>
       </c>
@@ -11575,8 +12411,14 @@
       <c r="AA132" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB132" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC132" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>62</v>
       </c>
@@ -11658,8 +12500,14 @@
       <c r="AA133" s="2">
         <v>46</v>
       </c>
-    </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB133" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC133" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>63</v>
       </c>
@@ -11741,8 +12589,14 @@
       <c r="AA134" s="2">
         <v>8338</v>
       </c>
-    </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB134" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC134" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>64</v>
       </c>
@@ -11824,8 +12678,14 @@
       <c r="AA135" s="2">
         <v>1335</v>
       </c>
-    </row>
-    <row r="136" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB135" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC135" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>65</v>
       </c>
@@ -11907,8 +12767,14 @@
       <c r="AA136" s="2">
         <v>4878</v>
       </c>
-    </row>
-    <row r="137" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB136" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC136" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>66</v>
       </c>
@@ -11990,8 +12856,14 @@
       <c r="AA137" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB137" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC137" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>67</v>
       </c>
@@ -12073,8 +12945,14 @@
       <c r="AA138" s="2">
         <v>846</v>
       </c>
-    </row>
-    <row r="139" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB138" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC138" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>68</v>
       </c>
@@ -12156,8 +13034,14 @@
       <c r="AA139" s="2">
         <v>538</v>
       </c>
-    </row>
-    <row r="140" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB139" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC139" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>69</v>
       </c>
@@ -12239,8 +13123,14 @@
       <c r="AA140" s="2">
         <v>9159</v>
       </c>
-    </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB140" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC140" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="141" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>70</v>
       </c>
@@ -12322,8 +13212,14 @@
       <c r="AA141" s="2">
         <v>279</v>
       </c>
-    </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB141" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC141" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="142" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>71</v>
       </c>
@@ -12405,8 +13301,14 @@
       <c r="AA142" s="2">
         <v>391</v>
       </c>
-    </row>
-    <row r="143" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB142" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC142" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="143" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>75</v>
       </c>
@@ -12488,8 +13390,14 @@
       <c r="AA143" s="2">
         <v>298065</v>
       </c>
-    </row>
-    <row r="144" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB143" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC143" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="144" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>26</v>
       </c>
@@ -12571,8 +13479,14 @@
       <c r="AA144" s="2">
         <v>30175</v>
       </c>
-    </row>
-    <row r="145" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB144" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC144" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="145" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>27</v>
       </c>
@@ -12654,8 +13568,14 @@
       <c r="AA145" s="2">
         <v>3232</v>
       </c>
-    </row>
-    <row r="146" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB145" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC145" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="146" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>28</v>
       </c>
@@ -12737,8 +13657,14 @@
       <c r="AA146" s="2">
         <v>4373</v>
       </c>
-    </row>
-    <row r="147" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB146" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC146" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="147" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>29</v>
       </c>
@@ -12820,8 +13746,14 @@
       <c r="AA147" s="2">
         <v>2458</v>
       </c>
-    </row>
-    <row r="148" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB147" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC147" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="148" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>30</v>
       </c>
@@ -12903,8 +13835,14 @@
       <c r="AA148" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB148" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC148" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="149" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>31</v>
       </c>
@@ -12986,8 +13924,14 @@
       <c r="AA149" s="2">
         <v>8451</v>
       </c>
-    </row>
-    <row r="150" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB149" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC149" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="150" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>32</v>
       </c>
@@ -13069,8 +14013,14 @@
       <c r="AA150" s="2">
         <v>1967</v>
       </c>
-    </row>
-    <row r="151" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB150" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC150" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="151" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>33</v>
       </c>
@@ -13152,8 +14102,14 @@
       <c r="AA151" s="2">
         <v>30349</v>
       </c>
-    </row>
-    <row r="152" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB151" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC151" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="152" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>34</v>
       </c>
@@ -13235,8 +14191,14 @@
       <c r="AA152" s="2">
         <v>33777</v>
       </c>
-    </row>
-    <row r="153" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB152" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC152" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="153" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>35</v>
       </c>
@@ -13318,8 +14280,14 @@
       <c r="AA153" s="2">
         <v>2847</v>
       </c>
-    </row>
-    <row r="154" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB153" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC153" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="154" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>36</v>
       </c>
@@ -13401,8 +14369,14 @@
       <c r="AA154" s="2">
         <v>8921</v>
       </c>
-    </row>
-    <row r="155" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB154" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC154" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="155" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>37</v>
       </c>
@@ -13484,8 +14458,14 @@
       <c r="AA155" s="2">
         <v>23412</v>
       </c>
-    </row>
-    <row r="156" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB155" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC155" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="156" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>38</v>
       </c>
@@ -13567,8 +14547,14 @@
       <c r="AA156" s="2">
         <v>7797</v>
       </c>
-    </row>
-    <row r="157" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB156" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC156" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="157" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>39</v>
       </c>
@@ -13650,8 +14636,14 @@
       <c r="AA157" s="2">
         <v>885</v>
       </c>
-    </row>
-    <row r="158" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB157" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC157" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="158" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>40</v>
       </c>
@@ -13733,8 +14725,14 @@
       <c r="AA158" s="2">
         <v>2233</v>
       </c>
-    </row>
-    <row r="159" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB158" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC158" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="159" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>41</v>
       </c>
@@ -13816,8 +14814,14 @@
       <c r="AA159" s="2">
         <v>1626</v>
       </c>
-    </row>
-    <row r="160" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB159" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC159" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="160" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>42</v>
       </c>
@@ -13899,8 +14903,14 @@
       <c r="AA160" s="2">
         <v>1192</v>
       </c>
-    </row>
-    <row r="161" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB160" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC160" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="161" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>43</v>
       </c>
@@ -13982,8 +14992,14 @@
       <c r="AA161" s="2">
         <v>2500</v>
       </c>
-    </row>
-    <row r="162" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB161" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC161" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="162" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>44</v>
       </c>
@@ -14065,8 +15081,14 @@
       <c r="AA162" s="2">
         <v>3722</v>
       </c>
-    </row>
-    <row r="163" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB162" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC162" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="163" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>45</v>
       </c>
@@ -14148,8 +15170,14 @@
       <c r="AA163" s="2">
         <v>3799</v>
       </c>
-    </row>
-    <row r="164" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB163" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC163" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="164" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>46</v>
       </c>
@@ -14231,8 +15259,14 @@
       <c r="AA164" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="165" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB164" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC164" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="165" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>47</v>
       </c>
@@ -14314,8 +15348,14 @@
       <c r="AA165" s="2">
         <v>20777</v>
       </c>
-    </row>
-    <row r="166" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB165" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC165" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="166" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>48</v>
       </c>
@@ -14397,8 +15437,14 @@
       <c r="AA166" s="2">
         <v>18975</v>
       </c>
-    </row>
-    <row r="167" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB166" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC166" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="167" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>49</v>
       </c>
@@ -14480,8 +15526,14 @@
       <c r="AA167" s="2">
         <v>4204</v>
       </c>
-    </row>
-    <row r="168" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB167" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC167" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="168" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>50</v>
       </c>
@@ -14563,8 +15615,14 @@
       <c r="AA168" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="169" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB168" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC168" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="169" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>51</v>
       </c>
@@ -14646,8 +15704,14 @@
       <c r="AA169" s="2">
         <v>1938</v>
       </c>
-    </row>
-    <row r="170" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB169" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC169" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="170" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>52</v>
       </c>
@@ -14729,8 +15793,14 @@
       <c r="AA170" s="2">
         <v>7863</v>
       </c>
-    </row>
-    <row r="171" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB170" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC170" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="171" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>53</v>
       </c>
@@ -14812,8 +15882,14 @@
       <c r="AA171" s="2">
         <v>3877</v>
       </c>
-    </row>
-    <row r="172" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB171" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC171" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="172" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>54</v>
       </c>
@@ -14895,8 +15971,14 @@
       <c r="AA172" s="2">
         <v>579</v>
       </c>
-    </row>
-    <row r="173" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB172" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC172" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="173" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>55</v>
       </c>
@@ -14978,8 +16060,14 @@
       <c r="AA173" s="2">
         <v>6161</v>
       </c>
-    </row>
-    <row r="174" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB173" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC173" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="174" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>56</v>
       </c>
@@ -15061,8 +16149,14 @@
       <c r="AA174" s="2">
         <v>10063</v>
       </c>
-    </row>
-    <row r="175" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB174" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC174" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="175" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>57</v>
       </c>
@@ -15144,8 +16238,14 @@
       <c r="AA175" s="2">
         <v>2022</v>
       </c>
-    </row>
-    <row r="176" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB175" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC175" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="176" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>58</v>
       </c>
@@ -15227,8 +16327,14 @@
       <c r="AA176" s="2">
         <v>5165</v>
       </c>
-    </row>
-    <row r="177" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB176" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC176" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="177" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>59</v>
       </c>
@@ -15310,8 +16416,14 @@
       <c r="AA177" s="2">
         <v>157</v>
       </c>
-    </row>
-    <row r="178" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB177" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC177" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="178" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>60</v>
       </c>
@@ -15393,8 +16505,14 @@
       <c r="AA178" s="2">
         <v>57</v>
       </c>
-    </row>
-    <row r="179" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB178" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC178" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="179" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>61</v>
       </c>
@@ -15476,8 +16594,14 @@
       <c r="AA179" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="180" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB179" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC179" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="180" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>62</v>
       </c>
@@ -15559,8 +16683,14 @@
       <c r="AA180" s="2">
         <v>109</v>
       </c>
-    </row>
-    <row r="181" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB180" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC180" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="181" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>63</v>
       </c>
@@ -15642,8 +16772,14 @@
       <c r="AA181" s="2">
         <v>13551</v>
       </c>
-    </row>
-    <row r="182" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB181" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC181" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="182" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>64</v>
       </c>
@@ -15725,8 +16861,14 @@
       <c r="AA182" s="2">
         <v>2993</v>
       </c>
-    </row>
-    <row r="183" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB182" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC182" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="183" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>65</v>
       </c>
@@ -15808,8 +16950,14 @@
       <c r="AA183" s="2">
         <v>6287</v>
       </c>
-    </row>
-    <row r="184" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB183" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC183" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="184" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>66</v>
       </c>
@@ -15891,8 +17039,14 @@
       <c r="AA184" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB184" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC184" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="185" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>67</v>
       </c>
@@ -15974,8 +17128,14 @@
       <c r="AA185" s="2">
         <v>2182</v>
       </c>
-    </row>
-    <row r="186" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB185" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC185" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="186" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>68</v>
       </c>
@@ -16057,8 +17217,14 @@
       <c r="AA186" s="2">
         <v>1938</v>
       </c>
-    </row>
-    <row r="187" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB186" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC186" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="187" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>69</v>
       </c>
@@ -16140,8 +17306,14 @@
       <c r="AA187" s="2">
         <v>14336</v>
       </c>
-    </row>
-    <row r="188" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB187" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC187" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="188" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>70</v>
       </c>
@@ -16223,8 +17395,14 @@
       <c r="AA188" s="2">
         <v>439</v>
       </c>
-    </row>
-    <row r="189" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB188" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC188" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="189" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>71</v>
       </c>
@@ -16306,8 +17484,14 @@
       <c r="AA189" s="2">
         <v>608</v>
       </c>
-    </row>
-    <row r="190" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB189" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC189" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="190" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>76</v>
       </c>
@@ -16389,8 +17573,14 @@
       <c r="AA190" s="2">
         <v>377887</v>
       </c>
-    </row>
-    <row r="191" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB190" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC190" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="191" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>26</v>
       </c>
@@ -16472,8 +17662,14 @@
       <c r="AA191" s="2">
         <v>40554</v>
       </c>
-    </row>
-    <row r="192" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB191" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC191" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="192" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>27</v>
       </c>
@@ -16555,8 +17751,14 @@
       <c r="AA192" s="2">
         <v>4008</v>
       </c>
-    </row>
-    <row r="193" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB192" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC192" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="193" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>28</v>
       </c>
@@ -16638,8 +17840,14 @@
       <c r="AA193" s="2">
         <v>5876</v>
       </c>
-    </row>
-    <row r="194" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB193" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC193" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="194" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>29</v>
       </c>
@@ -16721,8 +17929,14 @@
       <c r="AA194" s="2">
         <v>1997</v>
       </c>
-    </row>
-    <row r="195" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB194" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC194" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="195" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>30</v>
       </c>
@@ -16804,8 +18018,14 @@
       <c r="AA195" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB195" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC195" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="196" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>31</v>
       </c>
@@ -16887,8 +18107,14 @@
       <c r="AA196" s="2">
         <v>11656</v>
       </c>
-    </row>
-    <row r="197" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB196" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC196" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="197" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>32</v>
       </c>
@@ -16970,8 +18196,14 @@
       <c r="AA197" s="2">
         <v>2043</v>
       </c>
-    </row>
-    <row r="198" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB197" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC197" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="198" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>33</v>
       </c>
@@ -17053,8 +18285,14 @@
       <c r="AA198" s="2">
         <v>22880</v>
       </c>
-    </row>
-    <row r="199" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB198" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC198" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="199" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>34</v>
       </c>
@@ -17136,8 +18374,14 @@
       <c r="AA199" s="2">
         <v>48854</v>
       </c>
-    </row>
-    <row r="200" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB199" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC199" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="200" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>35</v>
       </c>
@@ -17219,8 +18463,14 @@
       <c r="AA200" s="2">
         <v>3109</v>
       </c>
-    </row>
-    <row r="201" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB200" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC200" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="201" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>36</v>
       </c>
@@ -17302,8 +18552,14 @@
       <c r="AA201" s="2">
         <v>10901</v>
       </c>
-    </row>
-    <row r="202" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB201" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC201" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="202" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>37</v>
       </c>
@@ -17385,8 +18641,14 @@
       <c r="AA202" s="2">
         <v>27604</v>
       </c>
-    </row>
-    <row r="203" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB202" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC202" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="203" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>38</v>
       </c>
@@ -17468,8 +18730,14 @@
       <c r="AA203" s="2">
         <v>8108</v>
       </c>
-    </row>
-    <row r="204" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB203" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC203" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="204" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>39</v>
       </c>
@@ -17551,8 +18819,14 @@
       <c r="AA204" s="2">
         <v>1612</v>
       </c>
-    </row>
-    <row r="205" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB204" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC204" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="205" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>40</v>
       </c>
@@ -17634,8 +18908,14 @@
       <c r="AA205" s="2">
         <v>3592</v>
       </c>
-    </row>
-    <row r="206" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB205" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC205" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="206" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>41</v>
       </c>
@@ -17717,8 +18997,14 @@
       <c r="AA206" s="2">
         <v>2401</v>
       </c>
-    </row>
-    <row r="207" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB206" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC206" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="207" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>42</v>
       </c>
@@ -17800,8 +19086,14 @@
       <c r="AA207" s="2">
         <v>1970</v>
       </c>
-    </row>
-    <row r="208" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB207" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC207" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="208" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>43</v>
       </c>
@@ -17883,8 +19175,14 @@
       <c r="AA208" s="2">
         <v>3468</v>
       </c>
-    </row>
-    <row r="209" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB208" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC208" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="209" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>44</v>
       </c>
@@ -17966,8 +19264,14 @@
       <c r="AA209" s="2">
         <v>3887</v>
       </c>
-    </row>
-    <row r="210" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB209" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC209" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="210" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>45</v>
       </c>
@@ -18049,8 +19353,14 @@
       <c r="AA210" s="2">
         <v>4621</v>
       </c>
-    </row>
-    <row r="211" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB210" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC210" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="211" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>46</v>
       </c>
@@ -18132,8 +19442,14 @@
       <c r="AA211" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="212" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB211" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC211" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="212" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>47</v>
       </c>
@@ -18215,8 +19531,14 @@
       <c r="AA212" s="2">
         <v>26221</v>
       </c>
-    </row>
-    <row r="213" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB212" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC212" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="213" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>48</v>
       </c>
@@ -18298,8 +19620,14 @@
       <c r="AA213" s="2">
         <v>27337</v>
       </c>
-    </row>
-    <row r="214" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB213" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC213" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="214" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>49</v>
       </c>
@@ -18381,8 +19709,14 @@
       <c r="AA214" s="2">
         <v>7104</v>
       </c>
-    </row>
-    <row r="215" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB214" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC214" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="215" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>50</v>
       </c>
@@ -18464,8 +19798,14 @@
       <c r="AA215" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="216" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB215" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC215" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="216" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>51</v>
       </c>
@@ -18547,8 +19887,14 @@
       <c r="AA216" s="2">
         <v>1971</v>
       </c>
-    </row>
-    <row r="217" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB216" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC216" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="217" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>52</v>
       </c>
@@ -18630,8 +19976,14 @@
       <c r="AA217" s="2">
         <v>8723</v>
       </c>
-    </row>
-    <row r="218" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB217" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC217" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="218" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>53</v>
       </c>
@@ -18713,8 +20065,14 @@
       <c r="AA218" s="2">
         <v>5239</v>
       </c>
-    </row>
-    <row r="219" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB218" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC218" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="219" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>54</v>
       </c>
@@ -18796,8 +20154,14 @@
       <c r="AA219" s="2">
         <v>1262</v>
       </c>
-    </row>
-    <row r="220" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB219" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC219" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="220" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>55</v>
       </c>
@@ -18879,8 +20243,14 @@
       <c r="AA220" s="2">
         <v>7523</v>
       </c>
-    </row>
-    <row r="221" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB220" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC220" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="221" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>56</v>
       </c>
@@ -18962,8 +20332,14 @@
       <c r="AA221" s="2">
         <v>11054</v>
       </c>
-    </row>
-    <row r="222" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB221" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC221" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="222" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>57</v>
       </c>
@@ -19045,8 +20421,14 @@
       <c r="AA222" s="2">
         <v>2648</v>
       </c>
-    </row>
-    <row r="223" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB222" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC222" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="223" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>58</v>
       </c>
@@ -19128,8 +20510,14 @@
       <c r="AA223" s="2">
         <v>6428</v>
       </c>
-    </row>
-    <row r="224" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB223" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC223" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="224" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>59</v>
       </c>
@@ -19211,8 +20599,14 @@
       <c r="AA224" s="2">
         <v>1061</v>
       </c>
-    </row>
-    <row r="225" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB224" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC224" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="225" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>60</v>
       </c>
@@ -19294,8 +20688,14 @@
       <c r="AA225" s="2">
         <v>587</v>
       </c>
-    </row>
-    <row r="226" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB225" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC225" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="226" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>61</v>
       </c>
@@ -19377,8 +20777,14 @@
       <c r="AA226" s="2">
         <v>160</v>
       </c>
-    </row>
-    <row r="227" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB226" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC226" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="227" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>62</v>
       </c>
@@ -19460,8 +20866,14 @@
       <c r="AA227" s="2">
         <v>179</v>
       </c>
-    </row>
-    <row r="228" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB227" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC227" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="228" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>63</v>
       </c>
@@ -19543,8 +20955,14 @@
       <c r="AA228" s="2">
         <v>16153</v>
       </c>
-    </row>
-    <row r="229" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB228" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC228" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="229" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>64</v>
       </c>
@@ -19626,8 +21044,14 @@
       <c r="AA229" s="2">
         <v>5138</v>
       </c>
-    </row>
-    <row r="230" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB229" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC229" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="230" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>65</v>
       </c>
@@ -19709,8 +21133,14 @@
       <c r="AA230" s="2">
         <v>8011</v>
       </c>
-    </row>
-    <row r="231" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB230" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC230" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="231" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>66</v>
       </c>
@@ -19792,8 +21222,14 @@
       <c r="AA231" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB231" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC231" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="232" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>67</v>
       </c>
@@ -19875,8 +21311,14 @@
       <c r="AA232" s="2">
         <v>1997</v>
       </c>
-    </row>
-    <row r="233" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB232" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC232" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="233" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>68</v>
       </c>
@@ -19958,8 +21400,14 @@
       <c r="AA233" s="2">
         <v>8036</v>
       </c>
-    </row>
-    <row r="234" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB233" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC233" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="234" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>69</v>
       </c>
@@ -20041,8 +21489,14 @@
       <c r="AA234" s="2">
         <v>20216</v>
       </c>
-    </row>
-    <row r="235" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB234" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC234" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="235" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>70</v>
       </c>
@@ -20124,8 +21578,14 @@
       <c r="AA235" s="2">
         <v>831</v>
       </c>
-    </row>
-    <row r="236" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB235" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC235" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="236" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>71</v>
       </c>
@@ -20207,8 +21667,14 @@
       <c r="AA236" s="2">
         <v>828</v>
       </c>
-    </row>
-    <row r="237" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB236" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC236" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="237" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>77</v>
       </c>
@@ -20290,8 +21756,14 @@
       <c r="AA237" s="2">
         <v>550020</v>
       </c>
-    </row>
-    <row r="238" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB237" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC237" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="238" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>26</v>
       </c>
@@ -20373,8 +21845,14 @@
       <c r="AA238" s="2">
         <v>54698</v>
       </c>
-    </row>
-    <row r="239" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB238" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC238" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="239" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>27</v>
       </c>
@@ -20456,8 +21934,14 @@
       <c r="AA239" s="2">
         <v>5915</v>
       </c>
-    </row>
-    <row r="240" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB239" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC239" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="240" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>28</v>
       </c>
@@ -20539,8 +22023,14 @@
       <c r="AA240" s="2">
         <v>8593</v>
       </c>
-    </row>
-    <row r="241" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB240" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC240" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="241" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>29</v>
       </c>
@@ -20622,8 +22112,14 @@
       <c r="AA241" s="2">
         <v>1498</v>
       </c>
-    </row>
-    <row r="242" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB241" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC241" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="242" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>30</v>
       </c>
@@ -20705,8 +22201,14 @@
       <c r="AA242" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="243" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB242" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC242" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="243" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>31</v>
       </c>
@@ -20788,8 +22290,14 @@
       <c r="AA243" s="2">
         <v>21521</v>
       </c>
-    </row>
-    <row r="244" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB243" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC243" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="244" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>32</v>
       </c>
@@ -20871,8 +22379,14 @@
       <c r="AA244" s="2">
         <v>3548</v>
       </c>
-    </row>
-    <row r="245" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB244" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC244" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="245" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>33</v>
       </c>
@@ -20954,8 +22468,14 @@
       <c r="AA245" s="2">
         <v>9224</v>
       </c>
-    </row>
-    <row r="246" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB245" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC245" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="246" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>34</v>
       </c>
@@ -21037,8 +22557,14 @@
       <c r="AA246" s="2">
         <v>97045</v>
       </c>
-    </row>
-    <row r="247" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB246" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC246" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="247" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>35</v>
       </c>
@@ -21120,8 +22646,14 @@
       <c r="AA247" s="2">
         <v>5539</v>
       </c>
-    </row>
-    <row r="248" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB247" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC247" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="248" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>36</v>
       </c>
@@ -21203,8 +22735,14 @@
       <c r="AA248" s="2">
         <v>13834</v>
       </c>
-    </row>
-    <row r="249" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB248" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC248" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="249" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>37</v>
       </c>
@@ -21286,8 +22824,14 @@
       <c r="AA249" s="2">
         <v>32376</v>
       </c>
-    </row>
-    <row r="250" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB249" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC249" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="250" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>38</v>
       </c>
@@ -21369,8 +22913,14 @@
       <c r="AA250" s="2">
         <v>12365</v>
       </c>
-    </row>
-    <row r="251" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB250" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC250" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="251" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>39</v>
       </c>
@@ -21452,8 +23002,14 @@
       <c r="AA251" s="2">
         <v>1998</v>
       </c>
-    </row>
-    <row r="252" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB251" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC251" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="252" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>40</v>
       </c>
@@ -21535,8 +23091,14 @@
       <c r="AA252" s="2">
         <v>4095</v>
       </c>
-    </row>
-    <row r="253" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB252" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC252" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="253" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>41</v>
       </c>
@@ -21618,8 +23180,14 @@
       <c r="AA253" s="2">
         <v>2745</v>
       </c>
-    </row>
-    <row r="254" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB253" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC253" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="254" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>42</v>
       </c>
@@ -21701,8 +23269,14 @@
       <c r="AA254" s="2">
         <v>2850</v>
       </c>
-    </row>
-    <row r="255" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB254" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC254" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="255" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>43</v>
       </c>
@@ -21784,8 +23358,14 @@
       <c r="AA255" s="2">
         <v>6970</v>
       </c>
-    </row>
-    <row r="256" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB255" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC255" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="256" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>44</v>
       </c>
@@ -21867,8 +23447,14 @@
       <c r="AA256" s="2">
         <v>5459</v>
       </c>
-    </row>
-    <row r="257" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB256" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC256" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="257" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>45</v>
       </c>
@@ -21950,8 +23536,14 @@
       <c r="AA257" s="2">
         <v>5748</v>
       </c>
-    </row>
-    <row r="258" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB257" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC257" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="258" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>46</v>
       </c>
@@ -22033,8 +23625,14 @@
       <c r="AA258" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="259" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB258" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC258" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="259" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>47</v>
       </c>
@@ -22116,8 +23714,14 @@
       <c r="AA259" s="2">
         <v>36809</v>
       </c>
-    </row>
-    <row r="260" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB259" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC259" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="260" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>48</v>
       </c>
@@ -22199,8 +23803,14 @@
       <c r="AA260" s="2">
         <v>42069</v>
       </c>
-    </row>
-    <row r="261" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB260" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC260" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="261" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>49</v>
       </c>
@@ -22282,8 +23892,14 @@
       <c r="AA261" s="2">
         <v>10238</v>
       </c>
-    </row>
-    <row r="262" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB261" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC261" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="262" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
         <v>50</v>
       </c>
@@ -22365,8 +23981,14 @@
       <c r="AA262" s="2">
         <v>52</v>
       </c>
-    </row>
-    <row r="263" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB262" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC262" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="263" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>51</v>
       </c>
@@ -22448,8 +24070,14 @@
       <c r="AA263" s="2">
         <v>2730</v>
       </c>
-    </row>
-    <row r="264" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB263" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC263" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="264" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>52</v>
       </c>
@@ -22531,8 +24159,14 @@
       <c r="AA264" s="2">
         <v>10724</v>
       </c>
-    </row>
-    <row r="265" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB264" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC264" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="265" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>53</v>
       </c>
@@ -22614,8 +24248,14 @@
       <c r="AA265" s="2">
         <v>7197</v>
       </c>
-    </row>
-    <row r="266" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB265" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC265" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="266" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>54</v>
       </c>
@@ -22697,8 +24337,14 @@
       <c r="AA266" s="2">
         <v>8415</v>
       </c>
-    </row>
-    <row r="267" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB266" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC266" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="267" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>55</v>
       </c>
@@ -22780,8 +24426,14 @@
       <c r="AA267" s="2">
         <v>12279</v>
       </c>
-    </row>
-    <row r="268" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB267" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC267" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="268" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>56</v>
       </c>
@@ -22863,8 +24515,14 @@
       <c r="AA268" s="2">
         <v>15613</v>
       </c>
-    </row>
-    <row r="269" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB268" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC268" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="269" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>57</v>
       </c>
@@ -22946,8 +24604,14 @@
       <c r="AA269" s="2">
         <v>2713</v>
       </c>
-    </row>
-    <row r="270" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB269" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC269" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="270" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
         <v>58</v>
       </c>
@@ -23029,8 +24693,14 @@
       <c r="AA270" s="2">
         <v>11394</v>
       </c>
-    </row>
-    <row r="271" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB270" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC270" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="271" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
         <v>59</v>
       </c>
@@ -23112,8 +24782,14 @@
       <c r="AA271" s="2">
         <v>2233</v>
       </c>
-    </row>
-    <row r="272" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB271" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC271" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="272" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
         <v>60</v>
       </c>
@@ -23195,8 +24871,14 @@
       <c r="AA272" s="2">
         <v>2047</v>
       </c>
-    </row>
-    <row r="273" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB272" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC272" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="273" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
         <v>61</v>
       </c>
@@ -23278,8 +24960,14 @@
       <c r="AA273" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="274" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB273" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC273" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="274" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>62</v>
       </c>
@@ -23361,8 +25049,14 @@
       <c r="AA274" s="2">
         <v>463</v>
       </c>
-    </row>
-    <row r="275" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB274" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC274" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="275" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>63</v>
       </c>
@@ -23444,8 +25138,14 @@
       <c r="AA275" s="2">
         <v>28491</v>
       </c>
-    </row>
-    <row r="276" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB275" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC275" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="276" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>64</v>
       </c>
@@ -23527,8 +25227,14 @@
       <c r="AA276" s="2">
         <v>10250</v>
       </c>
-    </row>
-    <row r="277" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB276" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC276" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="277" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
         <v>65</v>
       </c>
@@ -23610,8 +25316,14 @@
       <c r="AA277" s="2">
         <v>10181</v>
       </c>
-    </row>
-    <row r="278" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB277" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC277" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="278" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>66</v>
       </c>
@@ -23693,8 +25405,14 @@
       <c r="AA278" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="279" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB278" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC278" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="279" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
         <v>67</v>
       </c>
@@ -23776,8 +25494,14 @@
       <c r="AA279" s="2">
         <v>3657</v>
       </c>
-    </row>
-    <row r="280" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB279" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC279" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="280" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>68</v>
       </c>
@@ -23859,8 +25583,14 @@
       <c r="AA280" s="2">
         <v>8688</v>
       </c>
-    </row>
-    <row r="281" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB280" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC280" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="281" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
         <v>69</v>
       </c>
@@ -23942,8 +25672,14 @@
       <c r="AA281" s="2">
         <v>25549</v>
       </c>
-    </row>
-    <row r="282" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB281" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC281" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="282" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
         <v>70</v>
       </c>
@@ -24025,8 +25761,14 @@
       <c r="AA282" s="2">
         <v>1051</v>
       </c>
-    </row>
-    <row r="283" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB282" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC282" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="283" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
         <v>71</v>
       </c>
@@ -24107,6 +25849,12 @@
       </c>
       <c r="AA283" s="2">
         <v>1146</v>
+      </c>
+      <c r="AB283" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC283" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rettede fejl i forsikring i faste priser
</commit_message>
<xml_diff>
--- a/Estimering/fastepriser.xlsx
+++ b/Estimering/fastepriser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rasmuskaslund/Documents/GitHub/SpecialeJR /Estimering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52F2CE6-C48B-E84E-936A-06632987F88D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDE47D7-39F2-DD40-AF95-28F539FC07B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1400" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FU05" sheetId="2" r:id="rId1"/>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1:AC283"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4680,7 +4680,7 @@
         <v>69</v>
       </c>
       <c r="B46" s="2">
-        <v>256</v>
+        <v>12547</v>
       </c>
       <c r="C46" s="2">
         <v>12547</v>

</xml_diff>